<commit_message>
Made changes to Dashboard suite
Made changes to Dashboard suite
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/CreateAccount.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/CreateAccount.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="129">
   <si>
     <t>TCID</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Email_Field_Blank</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>Password_Field_Blank</t>
@@ -672,7 +675,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
+      <selection activeCell="E9" activeCellId="0" pane="topLeft" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -717,79 +720,79 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="5">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="6">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="7">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="8">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="9">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="10">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="11">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.05" outlineLevel="0" r="12">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -824,13 +827,13 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -838,13 +841,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>4</v>
@@ -884,19 +887,19 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
@@ -904,19 +907,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>4</v>
@@ -957,19 +960,19 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
@@ -977,19 +980,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>4</v>
@@ -1026,13 +1029,13 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -1040,13 +1043,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>4</v>
@@ -1071,7 +1074,7 @@
   <dimension ref="1:110"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I12" activeCellId="0" pane="topLeft" sqref="I12"/>
+      <selection activeCell="D15" activeCellId="0" pane="topLeft" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1094,22 +1097,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
@@ -1117,17 +1120,17 @@
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="5"/>
     </row>
@@ -1136,17 +1139,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="5"/>
     </row>
@@ -1155,17 +1158,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G4" s="5"/>
     </row>
@@ -1174,16 +1177,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -1193,16 +1196,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1212,16 +1215,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -1231,19 +1234,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G8" s="5"/>
     </row>
@@ -1252,19 +1255,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="G9" s="5"/>
     </row>
@@ -1273,16 +1276,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -1292,17 +1295,17 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -1311,16 +1314,16 @@
         <v>3</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
@@ -1330,16 +1333,16 @@
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -1349,17 +1352,17 @@
         <v>3</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G14" s="5"/>
     </row>
@@ -1368,13 +1371,13 @@
         <v>3</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -1385,17 +1388,17 @@
         <v>5</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G16" s="7"/>
     </row>
@@ -1404,17 +1407,17 @@
         <v>5</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="0"/>
@@ -1471,17 +1474,17 @@
         <v>5</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="0"/>
@@ -1538,16 +1541,16 @@
         <v>5</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1605,16 +1608,16 @@
         <v>5</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="9"/>
@@ -1672,19 +1675,19 @@
         <v>5</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="0"/>
@@ -1741,19 +1744,19 @@
         <v>5</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="0"/>
@@ -1810,16 +1813,16 @@
         <v>5</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="9"/>
@@ -1877,17 +1880,17 @@
         <v>5</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="0"/>
@@ -1944,17 +1947,17 @@
         <v>5</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="0"/>
@@ -2011,13 +2014,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
@@ -2076,17 +2079,17 @@
         <v>6</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="0"/>
@@ -2143,17 +2146,17 @@
         <v>6</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G28" s="10"/>
     </row>
@@ -2162,17 +2165,17 @@
         <v>6</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G29" s="10"/>
     </row>
@@ -2181,16 +2184,16 @@
         <v>6</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -2248,16 +2251,16 @@
         <v>6</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -2267,19 +2270,19 @@
         <v>6</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G32" s="10"/>
     </row>
@@ -2288,19 +2291,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G33" s="10"/>
     </row>
@@ -2309,16 +2312,16 @@
         <v>6</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
@@ -2328,17 +2331,17 @@
         <v>6</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E35" s="10"/>
       <c r="F35" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G35" s="10"/>
     </row>
@@ -2347,13 +2350,13 @@
         <v>6</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
@@ -2361,189 +2364,189 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="37">
       <c r="A37" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G37" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="38">
       <c r="A38" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G38" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="39">
       <c r="A39" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G39" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="40">
       <c r="A40" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="41">
       <c r="A41" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="42">
       <c r="A42" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="43">
       <c r="A43" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G43" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="44">
       <c r="A44" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="45">
       <c r="A45" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G45" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="46">
       <c r="A46" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
@@ -2551,189 +2554,189 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="47">
       <c r="A47" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G47" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="48">
       <c r="A48" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E48" s="7"/>
       <c r="F48" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G48" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="49">
       <c r="A49" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G49" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="50">
       <c r="A50" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="51">
       <c r="A51" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="52">
       <c r="A52" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="53">
       <c r="A53" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G53" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="54">
       <c r="A54" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="55">
       <c r="A55" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G55" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="56">
       <c r="A56" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E56" s="9"/>
       <c r="F56" s="9"/>
@@ -2741,212 +2744,212 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="57">
       <c r="A57" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E57" s="10"/>
       <c r="F57" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G57" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="58">
       <c r="A58" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E58" s="10"/>
       <c r="F58" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G58" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="59">
       <c r="A59" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E59" s="10"/>
       <c r="F59" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G59" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="60">
       <c r="A60" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E60" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="61">
       <c r="A61" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E61" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G61" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="62">
       <c r="A62" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="63">
       <c r="A63" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G63" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="64">
       <c r="A64" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B64" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F64" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="G64" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="65">
       <c r="A65" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="66">
       <c r="A66" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E66" s="10"/>
       <c r="F66" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G66" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="67">
       <c r="A67" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
@@ -2954,212 +2957,212 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="68">
       <c r="A68" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G68" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="69">
       <c r="A69" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G69" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="70">
       <c r="A70" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G70" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="71">
       <c r="A71" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="72">
       <c r="A72" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="73">
       <c r="A73" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G73" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="74">
       <c r="A74" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G74" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="75">
       <c r="A75" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B75" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F75" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="G75" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="76">
       <c r="A76" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="77">
       <c r="A77" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E77" s="5"/>
       <c r="F77" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G77" s="6"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="78">
       <c r="A78" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
@@ -3167,210 +3170,210 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="79">
       <c r="A79" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E79" s="7"/>
       <c r="F79" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G79" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="80">
       <c r="A80" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E80" s="7"/>
       <c r="F80" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G80" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="81">
       <c r="A81" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E81" s="7"/>
       <c r="F81" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G81" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="82">
       <c r="A82" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="83">
       <c r="A83" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D83" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="84">
       <c r="A84" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D84" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="85">
       <c r="A85" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G85" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="86">
       <c r="A86" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B86" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F86" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F86" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="G86" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="87">
       <c r="A87" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="88">
       <c r="A88" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D88" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E88" s="7"/>
       <c r="F88" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G88" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="89">
       <c r="A89" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D89" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
@@ -3378,210 +3381,210 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="90">
       <c r="A90" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E90" s="10"/>
       <c r="F90" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G90" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="91">
       <c r="A91" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E91" s="10"/>
       <c r="F91" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G91" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="92">
       <c r="A92" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D92" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E92" s="10"/>
       <c r="F92" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G92" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="93">
       <c r="A93" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C93" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D93" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="94">
       <c r="A94" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D94" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F94" s="10"/>
       <c r="G94" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="95">
       <c r="A95" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="96">
       <c r="A96" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G96" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="97">
       <c r="A97" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D97" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G97" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="98">
       <c r="A98" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D98" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E98" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F98" s="10"/>
       <c r="G98" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="99">
       <c r="A99" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E99" s="10"/>
       <c r="F99" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G99" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="100">
       <c r="A100" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E100" s="12"/>
       <c r="F100" s="12"/>
@@ -3589,195 +3592,195 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="101">
       <c r="A101" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E101" s="5"/>
       <c r="F101" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G101" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="102">
       <c r="A102" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G102" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="103">
       <c r="A103" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E103" s="5"/>
       <c r="F103" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G103" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="104">
       <c r="A104" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F104" s="5"/>
       <c r="G104" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="105">
       <c r="A105" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F105" s="5"/>
       <c r="G105" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="106">
       <c r="A106" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G106" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="107">
       <c r="A107" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G107" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="108">
       <c r="A108" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G108" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="109">
       <c r="A109" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G109" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="110">
       <c r="A110" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E110" s="6"/>
       <c r="F110" s="6"/>
@@ -3816,16 +3819,16 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>2</v>
@@ -3833,16 +3836,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>4</v>
@@ -3881,16 +3884,16 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>2</v>
@@ -3898,16 +3901,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="2">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>4</v>
@@ -3946,16 +3949,16 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>2</v>
@@ -3963,16 +3966,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="2">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>4</v>
@@ -4011,16 +4014,16 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>2</v>
@@ -4028,16 +4031,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>4</v>
@@ -4080,16 +4083,16 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>2</v>
@@ -4097,16 +4100,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>4</v>
@@ -4146,19 +4149,19 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
@@ -4166,19 +4169,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>4</v>
@@ -4218,19 +4221,19 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="1">
       <c r="A1" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
@@ -4238,19 +4241,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.9" outlineLevel="0" r="2">
       <c r="A2" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Code changes to My Mojio
Code changes to My Mojio
</commit_message>
<xml_diff>
--- a/MyMojioWebsite/src/com/mojio/xls/CreateAccount.xlsx
+++ b/MyMojioWebsite/src/com/mojio/xls/CreateAccount.xlsx
@@ -236,7 +236,7 @@
     <t>Close the browser</t>
   </si>
   <si>
-    <t>closeBroswer</t>
+    <t>closebrowser</t>
   </si>
   <si>
     <t>Verify the user name blank error</t>
@@ -675,7 +675,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E9" activeCellId="0" pane="topLeft" sqref="E9"/>
+      <selection activeCell="E9" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -814,7 +814,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C13" activeCellId="0" pane="topLeft" sqref="C13"/>
+      <selection activeCell="C13" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -872,7 +872,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E10" activeCellId="0" pane="topLeft" sqref="E10"/>
+      <selection activeCell="E10" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -944,7 +944,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A46" activeCellId="0" pane="topLeft" sqref="A46"/>
+      <selection activeCell="A46" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B28" activeCellId="0" pane="topLeft" sqref="B28"/>
+      <selection activeCell="B28" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1073,8 +1073,8 @@
   </sheetPr>
   <dimension ref="1:110"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D15" activeCellId="0" pane="topLeft" sqref="D15"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A23" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D26" activeCellId="1" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3805,7 +3805,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="D2"/>
+      <selection activeCell="D2" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3870,7 +3870,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D8" activeCellId="0" pane="topLeft" sqref="D8"/>
+      <selection activeCell="D8" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -3935,7 +3935,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
+      <selection activeCell="C14" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -4000,7 +4000,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D10" activeCellId="0" pane="topLeft" sqref="D10"/>
+      <selection activeCell="D10" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4065,7 +4065,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B30" activeCellId="0" pane="topLeft" sqref="B30"/>
+      <selection activeCell="B30" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4134,7 +4134,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E8" activeCellId="0" pane="topLeft" sqref="E8"/>
+      <selection activeCell="E8" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4206,7 +4206,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E6" activeCellId="0" pane="topLeft" sqref="E6"/>
+      <selection activeCell="E6" activeCellId="10" pane="topLeft" sqref="D15 D26 D36 D46 D56 D67 D78 D89 D100 D110 E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>